<commit_message>
minor changes in xls file
</commit_message>
<xml_diff>
--- a/docs/schedule Beispiel.xlsx
+++ b/docs/schedule Beispiel.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joar806b\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni-Stoff\Winter 19-20\Problem Solving\Assignment_01\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3037DEC6-354C-461F-BB2B-1184BE3236BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-480" yWindow="428" windowWidth="17625" windowHeight="8347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,8 +25,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>opti</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>versuch</t>
+  </si>
+  <si>
+    <t>primitiv</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,19 +430,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E6:AL43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C6:AL53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="AN27" sqref="AN27"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AE52" sqref="AE52:AG52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="38" width="4.7109375" customWidth="1"/>
+    <col min="5" max="38" width="4.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="5:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:35" x14ac:dyDescent="0.45">
       <c r="E6" s="4">
         <v>0</v>
       </c>
@@ -445,7 +464,10 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
     </row>
-    <row r="7" spans="5:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:35" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
       <c r="E7" s="4">
         <v>1</v>
       </c>
@@ -462,7 +484,7 @@
       <c r="P7" s="1"/>
       <c r="AG7" s="2"/>
     </row>
-    <row r="8" spans="5:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:35" x14ac:dyDescent="0.45">
       <c r="E8" s="4">
         <v>2</v>
       </c>
@@ -478,7 +500,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="5:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:35" x14ac:dyDescent="0.45">
       <c r="E9" s="4">
         <v>3</v>
       </c>
@@ -497,7 +519,7 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="5:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:35" x14ac:dyDescent="0.45">
       <c r="E10" s="4">
         <v>4</v>
       </c>
@@ -510,7 +532,7 @@
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
     </row>
-    <row r="11" spans="5:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:35" x14ac:dyDescent="0.45">
       <c r="E11" s="4">
         <v>5</v>
       </c>
@@ -526,7 +548,7 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="5:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:35" x14ac:dyDescent="0.45">
       <c r="E12" s="4">
         <v>0</v>
       </c>
@@ -621,7 +643,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:37" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
       <c r="E17" s="4">
         <v>0</v>
       </c>
@@ -643,7 +668,7 @@
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
     </row>
-    <row r="18" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E18" s="4">
         <v>1</v>
       </c>
@@ -660,7 +685,7 @@
       <c r="P18" s="1"/>
       <c r="AG18" s="2"/>
     </row>
-    <row r="19" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E19" s="4">
         <v>2</v>
       </c>
@@ -676,7 +701,7 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E20" s="4">
         <v>3</v>
       </c>
@@ -695,7 +720,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E21" s="4">
         <v>4</v>
       </c>
@@ -708,7 +733,7 @@
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
     </row>
-    <row r="22" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E22" s="4">
         <v>5</v>
       </c>
@@ -724,7 +749,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E23" s="4">
         <v>0</v>
       </c>
@@ -819,7 +844,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E27" s="4">
         <v>0</v>
       </c>
@@ -841,7 +866,7 @@
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
     </row>
-    <row r="28" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E28" s="4">
         <v>1</v>
       </c>
@@ -858,7 +883,7 @@
       <c r="T28" s="1"/>
       <c r="AF28" s="2"/>
     </row>
-    <row r="29" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E29" s="4">
         <v>2</v>
       </c>
@@ -874,7 +899,7 @@
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
     </row>
-    <row r="30" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E30" s="4">
         <v>3</v>
       </c>
@@ -893,7 +918,7 @@
       <c r="AG30" s="1"/>
       <c r="AH30" s="1"/>
     </row>
-    <row r="31" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E31" s="4">
         <v>4</v>
       </c>
@@ -906,7 +931,7 @@
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
     </row>
-    <row r="32" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:37" x14ac:dyDescent="0.45">
       <c r="E32" s="4">
         <v>5</v>
       </c>
@@ -922,7 +947,7 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="5:38" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:38" x14ac:dyDescent="0.45">
       <c r="E33" s="4">
         <v>0</v>
       </c>
@@ -1017,7 +1042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="5:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:38" x14ac:dyDescent="0.45">
       <c r="E37" s="4">
         <v>0</v>
       </c>
@@ -1039,7 +1064,10 @@
       <c r="AD37" s="2"/>
       <c r="AE37" s="2"/>
     </row>
-    <row r="38" spans="5:38" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:38" x14ac:dyDescent="0.45">
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
       <c r="E38" s="4">
         <v>1</v>
       </c>
@@ -1056,7 +1084,7 @@
       <c r="T38" s="1"/>
       <c r="AF38" s="2"/>
     </row>
-    <row r="39" spans="5:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:38" x14ac:dyDescent="0.45">
       <c r="E39" s="4">
         <v>2</v>
       </c>
@@ -1072,7 +1100,7 @@
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
     </row>
-    <row r="40" spans="5:38" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:38" x14ac:dyDescent="0.45">
       <c r="E40" s="4">
         <v>3</v>
       </c>
@@ -1091,7 +1119,7 @@
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
     </row>
-    <row r="41" spans="5:38" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:38" x14ac:dyDescent="0.45">
       <c r="E41" s="4">
         <v>4</v>
       </c>
@@ -1104,7 +1132,7 @@
       <c r="AK41" s="3"/>
       <c r="AL41" s="3"/>
     </row>
-    <row r="42" spans="5:38" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:38" x14ac:dyDescent="0.45">
       <c r="E42" s="4">
         <v>5</v>
       </c>
@@ -1120,7 +1148,7 @@
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="5:38" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:38" x14ac:dyDescent="0.45">
       <c r="E43" s="4">
         <v>0</v>
       </c>
@@ -1213,6 +1241,225 @@
       </c>
       <c r="AI43" s="4">
         <v>30</v>
+      </c>
+      <c r="AJ43" s="4">
+        <v>31</v>
+      </c>
+      <c r="AK43" s="4">
+        <v>32</v>
+      </c>
+      <c r="AL43" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="3:38" x14ac:dyDescent="0.45">
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="4">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="X47" s="2"/>
+      <c r="Y47" s="2"/>
+      <c r="Z47" s="2"/>
+      <c r="AA47" s="2"/>
+      <c r="AB47" s="2"/>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="2"/>
+      <c r="AF47" s="2"/>
+    </row>
+    <row r="48" spans="3:38" x14ac:dyDescent="0.45">
+      <c r="E48" s="4">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="AG48" s="2"/>
+    </row>
+    <row r="49" spans="5:38" x14ac:dyDescent="0.45">
+      <c r="E49" s="4">
+        <v>2</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+    </row>
+    <row r="50" spans="5:38" x14ac:dyDescent="0.45">
+      <c r="E50" s="4">
+        <v>3</v>
+      </c>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AC50" s="1"/>
+      <c r="AD50" s="1"/>
+    </row>
+    <row r="51" spans="5:38" x14ac:dyDescent="0.45">
+      <c r="E51" s="4">
+        <v>4</v>
+      </c>
+      <c r="X51" s="3"/>
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="3"/>
+      <c r="AC51" s="3"/>
+      <c r="AD51" s="3"/>
+      <c r="AE51" s="3"/>
+    </row>
+    <row r="52" spans="5:38" x14ac:dyDescent="0.45">
+      <c r="E52" s="4">
+        <v>5</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
+      <c r="AE52" s="1"/>
+      <c r="AF52" s="1"/>
+      <c r="AG52" s="1"/>
+    </row>
+    <row r="53" spans="5:38" x14ac:dyDescent="0.45">
+      <c r="E53" s="4">
+        <v>0</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1</v>
+      </c>
+      <c r="G53" s="4">
+        <v>2</v>
+      </c>
+      <c r="H53" s="4">
+        <v>3</v>
+      </c>
+      <c r="I53" s="4">
+        <v>4</v>
+      </c>
+      <c r="J53" s="4">
+        <v>5</v>
+      </c>
+      <c r="K53" s="4">
+        <v>6</v>
+      </c>
+      <c r="L53" s="4">
+        <v>7</v>
+      </c>
+      <c r="M53" s="4">
+        <v>8</v>
+      </c>
+      <c r="N53" s="4">
+        <v>9</v>
+      </c>
+      <c r="O53" s="4">
+        <v>10</v>
+      </c>
+      <c r="P53" s="4">
+        <v>11</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>12</v>
+      </c>
+      <c r="R53" s="4">
+        <v>13</v>
+      </c>
+      <c r="S53" s="4">
+        <v>14</v>
+      </c>
+      <c r="T53" s="4">
+        <v>15</v>
+      </c>
+      <c r="U53" s="4">
+        <v>16</v>
+      </c>
+      <c r="V53" s="4">
+        <v>17</v>
+      </c>
+      <c r="W53" s="4">
+        <v>18</v>
+      </c>
+      <c r="X53" s="4">
+        <v>19</v>
+      </c>
+      <c r="Y53" s="4">
+        <v>20</v>
+      </c>
+      <c r="Z53" s="4">
+        <v>21</v>
+      </c>
+      <c r="AA53" s="4">
+        <v>22</v>
+      </c>
+      <c r="AB53" s="4">
+        <v>23</v>
+      </c>
+      <c r="AC53" s="4">
+        <v>24</v>
+      </c>
+      <c r="AD53" s="4">
+        <v>25</v>
+      </c>
+      <c r="AE53" s="4">
+        <v>26</v>
+      </c>
+      <c r="AF53" s="4">
+        <v>27</v>
+      </c>
+      <c r="AG53" s="4">
+        <v>28</v>
+      </c>
+      <c r="AH53" s="4">
+        <v>29</v>
+      </c>
+      <c r="AI53" s="4">
+        <v>30</v>
+      </c>
+      <c r="AJ53" s="4">
+        <v>31</v>
+      </c>
+      <c r="AK53" s="4">
+        <v>32</v>
+      </c>
+      <c r="AL53" s="4">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>